<commit_message>
Updates: docker-compose to version 2
</commit_message>
<xml_diff>
--- a/GCSG - Action Items (version 1).xlsx
+++ b/GCSG - Action Items (version 1).xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="99">
   <si>
     <t>SN</t>
   </si>
@@ -1390,6 +1390,24 @@
       </rPr>
       <t>_sync scheduler</t>
     </r>
+  </si>
+  <si>
+    <t>5.2.0</t>
+  </si>
+  <si>
+    <t>Declare all necesarry branch queues</t>
+  </si>
+  <si>
+    <t>CORP:agm_branch -&gt; CORP:agm_branch</t>
+  </si>
+  <si>
+    <t>agm_branch_boot</t>
+  </si>
+  <si>
+    <t>Done 5.2.1</t>
+  </si>
+  <si>
+    <t>DONE</t>
   </si>
 </sst>
 </file>
@@ -3656,30 +3674,34 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="5.33203125" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" style="15"/>
+    <col min="3" max="3" width="42.1640625" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.1640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="14.5" style="15"/>
+    <col min="5" max="5" width="23.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="14.5" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="15" t="s">
         <v>75</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="B2" s="15" t="s">
         <v>76</v>
       </c>
@@ -3687,7 +3709,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" s="15">
         <v>1</v>
       </c>
@@ -3697,8 +3719,11 @@
       <c r="C3" s="15" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="16">
         <v>2</v>
       </c>
@@ -3708,13 +3733,16 @@
       <c r="C4" s="15" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="B5" s="17" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" s="15">
         <v>3</v>
       </c>
@@ -3725,7 +3753,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7" s="15">
         <v>4</v>
       </c>
@@ -3735,8 +3763,11 @@
       <c r="C7" s="15" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" s="15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="15">
         <v>5</v>
       </c>
@@ -3746,8 +3777,11 @@
       <c r="C8" s="15" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" s="15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="15">
         <v>6</v>
       </c>
@@ -3758,7 +3792,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:4">
       <c r="A10" s="15">
         <v>7</v>
       </c>
@@ -3767,6 +3801,27 @@
       </c>
       <c r="C10" s="15" t="s">
         <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="B13" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="15" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -3784,7 +3839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B7"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>

</xml_diff>